<commit_message>
change to gooxml for reading xlsx files and improve the default values
</commit_message>
<xml_diff>
--- a/testfiles/Nummerliggare_2.xlsx
+++ b/testfiles/Nummerliggare_2.xlsx
@@ -170,12 +170,12 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -185,7 +185,7 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -193,7 +193,7 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -216,7 +216,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT($B$1, "-",TEXT(A5, "0000"))</f>
+        <f aca="false">_xlfn.CONCAT($C$1, "-",TEXT(A5, "0000"))</f>
         <v>P4567-0001</v>
       </c>
     </row>
@@ -228,7 +228,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="str">
-        <f aca="false">IF(B6="","",_xlfn.CONCAT($B$1, "-",TEXT(A6, "0000")))</f>
+        <f aca="false">IF(B6="","",_xlfn.CONCAT($C$1, "-",TEXT(A6, "0000")))</f>
         <v>P4567-0002</v>
       </c>
     </row>
@@ -240,7 +240,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="0" t="str">
-        <f aca="false">IF(B7="","",_xlfn.CONCAT($B$1, "-",TEXT(A7, "0000")))</f>
+        <f aca="false">IF(B7="","",_xlfn.CONCAT($C$1, "-",TEXT(A7, "0000")))</f>
         <v>P4567-0003</v>
       </c>
     </row>
@@ -252,7 +252,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="0" t="str">
-        <f aca="false">IF(B8="","",_xlfn.CONCAT($B$1, "-",TEXT(A8, "0000")))</f>
+        <f aca="false">IF(B8="","",_xlfn.CONCAT($C$1, "-",TEXT(A8, "0000")))</f>
         <v>P4567-0004</v>
       </c>
     </row>
@@ -264,7 +264,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="0" t="str">
-        <f aca="false">IF(B9="","",_xlfn.CONCAT($B$1, "-",TEXT(A9, "0000")))</f>
+        <f aca="false">IF(B9="","",_xlfn.CONCAT($C$1, "-",TEXT(A9, "0000")))</f>
         <v>P4567-0005</v>
       </c>
     </row>
@@ -276,7 +276,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="0" t="str">
-        <f aca="false">IF(B10="","",_xlfn.CONCAT($B$1, "-",TEXT(A10, "0000")))</f>
+        <f aca="false">IF(B10="","",_xlfn.CONCAT($C$1, "-",TEXT(A10, "0000")))</f>
         <v>P4567-0006</v>
       </c>
     </row>
@@ -288,7 +288,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="0" t="str">
-        <f aca="false">IF(B11="","",_xlfn.CONCAT($B$1, "-",TEXT(A11, "0000")))</f>
+        <f aca="false">IF(B11="","",_xlfn.CONCAT($C$1, "-",TEXT(A11, "0000")))</f>
         <v>P4567-0007</v>
       </c>
     </row>
@@ -300,7 +300,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="0" t="str">
-        <f aca="false">IF(B12="","",_xlfn.CONCAT($B$1, "-",TEXT(A12, "0000")))</f>
+        <f aca="false">IF(B12="","",_xlfn.CONCAT($C$1, "-",TEXT(A12, "0000")))</f>
         <v>P4567-0008</v>
       </c>
     </row>
@@ -312,7 +312,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="0" t="str">
-        <f aca="false">IF(B13="","",_xlfn.CONCAT($B$1, "-",TEXT(A13, "0000")))</f>
+        <f aca="false">IF(B13="","",_xlfn.CONCAT($C$1, "-",TEXT(A13, "0000")))</f>
         <v>P4567-0009</v>
       </c>
     </row>
@@ -324,7 +324,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="0" t="str">
-        <f aca="false">IF(B14="","",_xlfn.CONCAT($B$1, "-",TEXT(A14, "0000")))</f>
+        <f aca="false">IF(B14="","",_xlfn.CONCAT($C$1, "-",TEXT(A14, "0000")))</f>
         <v>P4567-0010</v>
       </c>
     </row>
@@ -333,7 +333,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="0" t="str">
-        <f aca="false">IF(B15="","",_xlfn.CONCAT($B$1, "-",TEXT(A15, "0000")))</f>
+        <f aca="false">IF(B15="","",_xlfn.CONCAT($C$1, "-",TEXT(A15, "0000")))</f>
         <v/>
       </c>
     </row>
@@ -342,7 +342,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="0" t="str">
-        <f aca="false">IF(B16="","",_xlfn.CONCAT($B$1, "-",TEXT(A16, "0000")))</f>
+        <f aca="false">IF(B16="","",_xlfn.CONCAT($C$1, "-",TEXT(A16, "0000")))</f>
         <v/>
       </c>
     </row>
@@ -351,7 +351,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="str">
-        <f aca="false">IF(B17="","",_xlfn.CONCAT($B$1, "-",TEXT(A17, "0000")))</f>
+        <f aca="false">IF(B17="","",_xlfn.CONCAT($C$1, "-",TEXT(A17, "0000")))</f>
         <v/>
       </c>
     </row>
@@ -360,97 +360,97 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="str">
-        <f aca="false">IF(B18="","",_xlfn.CONCAT($B$1, "-",TEXT(A18, "0000")))</f>
+        <f aca="false">IF(B18="","",_xlfn.CONCAT($C$1, "-",TEXT(A18, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="str">
-        <f aca="false">IF(B19="","",_xlfn.CONCAT($B$1, "-",TEXT(A19, "0000")))</f>
+        <f aca="false">IF(B19="","",_xlfn.CONCAT($C$1, "-",TEXT(A19, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="str">
-        <f aca="false">IF(B20="","",_xlfn.CONCAT($B$1, "-",TEXT(A20, "0000")))</f>
+        <f aca="false">IF(B20="","",_xlfn.CONCAT($C$1, "-",TEXT(A20, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="str">
-        <f aca="false">IF(B21="","",_xlfn.CONCAT($B$1, "-",TEXT(A21, "0000")))</f>
+        <f aca="false">IF(B21="","",_xlfn.CONCAT($C$1, "-",TEXT(A21, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="str">
-        <f aca="false">IF(B22="","",_xlfn.CONCAT($B$1, "-",TEXT(A22, "0000")))</f>
+        <f aca="false">IF(B22="","",_xlfn.CONCAT($C$1, "-",TEXT(A22, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="str">
-        <f aca="false">IF(B23="","",_xlfn.CONCAT($B$1, "-",TEXT(A23, "0000")))</f>
+        <f aca="false">IF(B23="","",_xlfn.CONCAT($C$1, "-",TEXT(A23, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="str">
-        <f aca="false">IF(B24="","",_xlfn.CONCAT($B$1, "-",TEXT(A24, "0000")))</f>
+        <f aca="false">IF(B24="","",_xlfn.CONCAT($C$1, "-",TEXT(A24, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="str">
-        <f aca="false">IF(B25="","",_xlfn.CONCAT($B$1, "-",TEXT(A25, "0000")))</f>
+        <f aca="false">IF(B25="","",_xlfn.CONCAT($C$1, "-",TEXT(A25, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="str">
-        <f aca="false">IF(B26="","",_xlfn.CONCAT($B$1, "-",TEXT(A26, "0000")))</f>
+        <f aca="false">IF(B26="","",_xlfn.CONCAT($C$1, "-",TEXT(A26, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="str">
-        <f aca="false">IF(B27="","",_xlfn.CONCAT($B$1, "-",TEXT(A27, "0000")))</f>
+        <f aca="false">IF(B27="","",_xlfn.CONCAT($C$1, "-",TEXT(A27, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="str">
-        <f aca="false">IF(B28="","",_xlfn.CONCAT($B$1, "-",TEXT(A28, "0000")))</f>
+        <f aca="false">IF(B28="","",_xlfn.CONCAT($C$1, "-",TEXT(A28, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="str">
-        <f aca="false">IF(B29="","",_xlfn.CONCAT($B$1, "-",TEXT(A29, "0000")))</f>
+        <f aca="false">IF(B29="","",_xlfn.CONCAT($C$1, "-",TEXT(A29, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="str">
-        <f aca="false">IF(B30="","",_xlfn.CONCAT($B$1, "-",TEXT(A30, "0000")))</f>
+        <f aca="false">IF(B30="","",_xlfn.CONCAT($C$1, "-",TEXT(A30, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="str">
-        <f aca="false">IF(B31="","",_xlfn.CONCAT($B$1, "-",TEXT(A31, "0000")))</f>
+        <f aca="false">IF(B31="","",_xlfn.CONCAT($C$1, "-",TEXT(A31, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="str">
-        <f aca="false">IF(B32="","",_xlfn.CONCAT($B$1, "-",TEXT(A32, "0000")))</f>
+        <f aca="false">IF(B32="","",_xlfn.CONCAT($C$1, "-",TEXT(A32, "0000")))</f>
         <v/>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="str">
-        <f aca="false">IF(B33="","",_xlfn.CONCAT($B$1, "-",TEXT(A33, "0000")))</f>
+        <f aca="false">IF(B33="","",_xlfn.CONCAT($C$1, "-",TEXT(A33, "0000")))</f>
         <v/>
       </c>
     </row>

</xml_diff>